<commit_message>
Add employee - CreateloginDetails
</commit_message>
<xml_diff>
--- a/src/resources/java/com/TestDataInputFiles/OrangeHRMTestData.xlsx
+++ b/src/resources/java/com/TestDataInputFiles/OrangeHRMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="4350" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="6000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="PIMEmployeeListPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Expected_LoginPage_Title</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Expected_LastName</t>
   </si>
   <si>
-    <t>Expected_EmpID</t>
-  </si>
-  <si>
     <t>Photograph</t>
   </si>
   <si>
@@ -248,47 +245,45 @@
     <t>auth/login</t>
   </si>
   <si>
-    <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>SKLakshmi</t>
   </si>
   <si>
+    <t>SKLakshmi@19</t>
+  </si>
+  <si>
     <t>SitaRamaK</t>
   </si>
   <si>
+    <t>SitaRamaK@19</t>
+  </si>
+  <si>
     <t>KarthikVLakshmi</t>
   </si>
   <si>
+    <t>KarthikVLaskshmi@19</t>
+  </si>
+  <si>
     <t>RamanaVenkataKrishna</t>
   </si>
   <si>
-    <t>SKLakshmi@19</t>
-  </si>
-  <si>
-    <t>SitaRamaK@19</t>
-  </si>
-  <si>
     <t>RamanaVenkataKrishna@19</t>
   </si>
   <si>
-    <t>KarthikVLaskshmi@19</t>
-  </si>
-  <si>
     <t>GeethaLucky</t>
   </si>
   <si>
     <t>GeethaLucky@19</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,14 +295,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,17 +317,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,25 +629,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -720,39 +704,15 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
       <c r="M2" t="s">
         <v>14</v>
       </c>
@@ -764,6 +724,42 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
       <c r="M3" t="s">
         <v>16</v>
       </c>
@@ -772,6 +768,9 @@
       </c>
       <c r="O3" t="s">
         <v>26</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -833,11 +832,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="40.5703125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,24 +938,23 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -976,13 +974,13 @@
         <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>53</v>
@@ -997,140 +995,130 @@
         <v>56</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
-        <v>70</v>
+      <c r="D5" t="s">
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
-        <v>73</v>
+      <c r="D6" t="s">
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>